<commit_message>
Inserindo informações de estado civil e escolaridade
</commit_message>
<xml_diff>
--- a/2014/Centro-Oeste/DISTRITO-FEDERAL/resultado.xlsx
+++ b/2014/Centro-Oeste/DISTRITO-FEDERAL/resultado.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:H135"/>
+  <dimension ref="A1:J135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -474,6 +474,16 @@
           <t>DS_GENERO</t>
         </is>
       </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>DS_ESTADO_CIVIL</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>DS_GRAU_INSTRUCAO</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -514,6 +524,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -554,6 +574,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -594,6 +624,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -634,6 +674,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -674,6 +724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -714,6 +774,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -754,6 +824,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -794,6 +874,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -834,6 +924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -874,6 +974,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -914,6 +1024,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -954,6 +1074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -994,6 +1124,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1034,6 +1174,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1074,6 +1224,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1114,6 +1274,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1154,6 +1324,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1194,6 +1374,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1234,6 +1424,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1274,6 +1474,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1314,6 +1524,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1354,6 +1574,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1394,6 +1624,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1434,6 +1674,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1474,6 +1724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1514,6 +1774,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1554,6 +1824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1594,6 +1874,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1634,6 +1924,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1674,6 +1974,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1714,6 +2024,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -1754,6 +2074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -1794,6 +2124,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1834,6 +2174,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1874,6 +2224,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1914,6 +2274,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1954,6 +2324,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -1994,6 +2374,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2034,6 +2424,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2074,6 +2474,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2114,6 +2524,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2154,6 +2574,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2194,6 +2624,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2234,6 +2674,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2274,6 +2724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2314,6 +2774,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2354,6 +2824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2394,6 +2874,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2434,6 +2924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2474,6 +2974,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2514,6 +3024,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2554,6 +3074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2594,6 +3124,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -2634,6 +3174,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2674,6 +3224,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2714,6 +3274,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -2754,6 +3324,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -2794,6 +3374,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -2834,6 +3424,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -2874,6 +3474,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -2914,6 +3524,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -2954,6 +3574,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -2994,6 +3624,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3034,6 +3674,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3074,6 +3724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3114,6 +3774,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3154,6 +3824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3194,6 +3874,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3234,6 +3924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3274,6 +3974,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -3314,6 +4024,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I72" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -3354,6 +4074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I73" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -3394,6 +4124,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I74" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -3434,6 +4174,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I75" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -3474,6 +4224,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I76" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -3514,6 +4274,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I77" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -3554,6 +4324,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I78" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -3594,6 +4374,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I79" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -3634,6 +4424,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I80" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -3674,6 +4474,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I81" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -3714,6 +4524,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I82" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -3754,6 +4574,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I83" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -3794,6 +4624,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I84" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -3834,6 +4674,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I85" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -3874,6 +4724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I86" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -3914,6 +4774,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I87" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -3954,6 +4824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I88" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -3994,6 +4874,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I89" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4034,6 +4924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I90" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4074,6 +4974,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I91" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -4114,6 +5024,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I92" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -4154,6 +5074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I93" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -4194,6 +5124,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I94" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -4234,6 +5174,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I95" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -4274,6 +5224,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I96" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -4314,6 +5274,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I97" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -4354,6 +5324,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I98" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -4394,6 +5374,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I99" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -4434,6 +5424,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I100" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -4474,6 +5474,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I101" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -4514,6 +5524,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I102" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -4554,6 +5574,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I103" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -4594,6 +5624,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I104" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -4634,6 +5674,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I105" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -4674,6 +5724,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I106" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -4714,6 +5774,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I107" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -4754,6 +5824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I108" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -4794,6 +5874,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I109" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -4834,6 +5924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I110" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -4874,6 +5974,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I111" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -4914,6 +6024,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I112" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -4954,6 +6074,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I113" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -4994,6 +6124,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I114" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -5034,6 +6174,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I115" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -5074,6 +6224,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I116" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -5114,6 +6274,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I117" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -5154,6 +6324,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I118" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -5194,6 +6374,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I119" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -5234,6 +6424,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I120" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -5274,6 +6474,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I121" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -5314,6 +6524,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I122" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -5354,6 +6574,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I123" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -5394,6 +6624,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I124" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -5434,6 +6674,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I125" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -5474,6 +6724,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I126" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -5514,6 +6774,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I127" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -5554,6 +6824,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I128" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -5594,6 +6874,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I129" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -5634,6 +6924,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I130" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -5674,6 +6974,16 @@
           <t>MASCULINO</t>
         </is>
       </c>
+      <c r="I131" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -5714,6 +7024,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I132" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -5754,6 +7074,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I133" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -5794,6 +7124,16 @@
           <t>FEMININO</t>
         </is>
       </c>
+      <c r="I134" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -5832,6 +7172,16 @@
       <c r="H135" t="inlineStr">
         <is>
           <t>MASCULINO</t>
+        </is>
+      </c>
+      <c r="I135" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
criando código de atualizar partidos
</commit_message>
<xml_diff>
--- a/2014/Centro-Oeste/DISTRITO-FEDERAL/resultado.xlsx
+++ b/2014/Centro-Oeste/DISTRITO-FEDERAL/resultado.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J135"/>
+  <dimension ref="A1:N135"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -476,12 +476,32 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>DS_ESTADO_CIVIL</t>
+          <t>DS_ESTADO_CIVIL_x</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>DS_GRAU_INSTRUCAO</t>
+          <t>DS_GRAU_INSTRUCAO_x</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>DS_ESTADO_CIVIL_y</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>DS_GRAU_INSTRUCAO_y</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>SQ_CANDIDATO</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>SG_PARTIDO</t>
         </is>
       </c>
     </row>
@@ -534,6 +554,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L2" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M2" t="n">
+        <v>70000000157</v>
+      </c>
+      <c r="N2" t="inlineStr">
+        <is>
+          <t>PCB</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -584,6 +622,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M3" t="n">
+        <v>70000000164</v>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>PSTU</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -634,6 +690,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L4" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M4" t="n">
+        <v>70000000165</v>
+      </c>
+      <c r="N4" t="inlineStr">
+        <is>
+          <t>PSTU</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -684,6 +758,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L5" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M5" t="n">
+        <v>70000000168</v>
+      </c>
+      <c r="N5" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -734,6 +826,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L6" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M6" t="n">
+        <v>70000000169</v>
+      </c>
+      <c r="N6" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -784,6 +894,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M7" t="n">
+        <v>70000000170</v>
+      </c>
+      <c r="N7" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -834,6 +962,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K8" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L8" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M8" t="n">
+        <v>70000000171</v>
+      </c>
+      <c r="N8" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -884,6 +1030,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K9" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M9" t="n">
+        <v>70000000172</v>
+      </c>
+      <c r="N9" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -934,6 +1098,24 @@
           <t>LÊ E ESCREVE</t>
         </is>
       </c>
+      <c r="K10" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L10" t="inlineStr">
+        <is>
+          <t>LÊ E ESCREVE</t>
+        </is>
+      </c>
+      <c r="M10" t="n">
+        <v>70000000173</v>
+      </c>
+      <c r="N10" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -984,6 +1166,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K11" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M11" t="n">
+        <v>70000000174</v>
+      </c>
+      <c r="N11" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1034,6 +1234,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K12" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L12" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M12" t="n">
+        <v>70000000175</v>
+      </c>
+      <c r="N12" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1084,6 +1302,24 @@
           <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
         </is>
       </c>
+      <c r="K13" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L13" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M13" t="n">
+        <v>70000000176</v>
+      </c>
+      <c r="N13" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1134,6 +1370,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K14" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L14" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M14" t="n">
+        <v>70000000177</v>
+      </c>
+      <c r="N14" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1184,6 +1438,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K15" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M15" t="n">
+        <v>70000000178</v>
+      </c>
+      <c r="N15" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1234,6 +1506,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K16" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M16" t="n">
+        <v>70000000179</v>
+      </c>
+      <c r="N16" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1284,6 +1574,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K17" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M17" t="n">
+        <v>70000000180</v>
+      </c>
+      <c r="N17" t="inlineStr">
+        <is>
+          <t>PSOL</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1334,6 +1642,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K18" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M18" t="n">
+        <v>70000000439</v>
+      </c>
+      <c r="N18" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1384,6 +1710,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K19" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M19" t="n">
+        <v>70000000440</v>
+      </c>
+      <c r="N19" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1434,6 +1778,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K20" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M20" t="n">
+        <v>70000000441</v>
+      </c>
+      <c r="N20" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1484,6 +1846,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K21" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L21" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M21" t="n">
+        <v>70000000442</v>
+      </c>
+      <c r="N21" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1534,6 +1914,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K22" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L22" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M22" t="n">
+        <v>70000000443</v>
+      </c>
+      <c r="N22" t="inlineStr">
+        <is>
+          <t>SD</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -1584,6 +1982,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K23" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L23" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M23" t="n">
+        <v>70000000444</v>
+      </c>
+      <c r="N23" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -1634,6 +2050,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K24" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L24" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M24" t="n">
+        <v>70000000445</v>
+      </c>
+      <c r="N24" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -1684,6 +2118,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K25" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L25" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M25" t="n">
+        <v>70000000446</v>
+      </c>
+      <c r="N25" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -1734,6 +2186,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K26" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M26" t="n">
+        <v>70000000447</v>
+      </c>
+      <c r="N26" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1784,6 +2254,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K27" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M27" t="n">
+        <v>70000000448</v>
+      </c>
+      <c r="N27" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1834,6 +2322,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K28" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M28" t="n">
+        <v>70000000449</v>
+      </c>
+      <c r="N28" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1884,6 +2390,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K29" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M29" t="n">
+        <v>70000000450</v>
+      </c>
+      <c r="N29" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1934,6 +2458,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K30" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M30" t="n">
+        <v>70000000451</v>
+      </c>
+      <c r="N30" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1984,6 +2526,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K31" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M31" t="n">
+        <v>70000000452</v>
+      </c>
+      <c r="N31" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -2034,6 +2594,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K32" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L32" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M32" t="n">
+        <v>70000000453</v>
+      </c>
+      <c r="N32" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -2084,6 +2662,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K33" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M33" t="n">
+        <v>70000000454</v>
+      </c>
+      <c r="N33" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2134,6 +2730,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K34" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M34" t="n">
+        <v>70000000455</v>
+      </c>
+      <c r="N34" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2184,6 +2798,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K35" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M35" t="n">
+        <v>70000000456</v>
+      </c>
+      <c r="N35" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2234,6 +2866,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K36" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M36" t="n">
+        <v>70000000457</v>
+      </c>
+      <c r="N36" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2284,6 +2934,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K37" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M37" t="n">
+        <v>70000000458</v>
+      </c>
+      <c r="N37" t="inlineStr">
+        <is>
+          <t>PSB</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2334,6 +3002,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K38" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M38" t="n">
+        <v>70000000459</v>
+      </c>
+      <c r="N38" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2384,6 +3070,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K39" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M39" t="n">
+        <v>70000000460</v>
+      </c>
+      <c r="N39" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2434,6 +3138,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K40" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L40" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M40" t="n">
+        <v>70000000461</v>
+      </c>
+      <c r="N40" t="inlineStr">
+        <is>
+          <t>PSD</t>
+        </is>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -2484,6 +3206,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K41" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M41" t="n">
+        <v>70000000582</v>
+      </c>
+      <c r="N41" t="inlineStr">
+        <is>
+          <t>PDT</t>
+        </is>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2534,6 +3274,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M42" t="n">
+        <v>70000000657</v>
+      </c>
+      <c r="N42" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2584,6 +3342,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M43" t="n">
+        <v>70000000658</v>
+      </c>
+      <c r="N43" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2634,6 +3410,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K44" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M44" t="n">
+        <v>70000000659</v>
+      </c>
+      <c r="N44" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2684,6 +3478,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K45" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M45" t="n">
+        <v>70000000660</v>
+      </c>
+      <c r="N45" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2734,6 +3546,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K46" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M46" t="n">
+        <v>70000000661</v>
+      </c>
+      <c r="N46" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2784,6 +3614,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K47" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M47" t="n">
+        <v>70000000662</v>
+      </c>
+      <c r="N47" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2834,6 +3682,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K48" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M48" t="n">
+        <v>70000000663</v>
+      </c>
+      <c r="N48" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2884,6 +3750,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K49" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M49" t="n">
+        <v>70000000664</v>
+      </c>
+      <c r="N49" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2934,6 +3818,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K50" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M50" t="n">
+        <v>70000000665</v>
+      </c>
+      <c r="N50" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2984,6 +3886,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K51" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M51" t="n">
+        <v>70000000666</v>
+      </c>
+      <c r="N51" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -3034,6 +3954,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K52" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M52" t="n">
+        <v>70000000667</v>
+      </c>
+      <c r="N52" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -3084,6 +4022,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K53" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M53" t="n">
+        <v>70000000668</v>
+      </c>
+      <c r="N53" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -3134,6 +4090,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K54" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L54" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M54" t="n">
+        <v>70000000669</v>
+      </c>
+      <c r="N54" t="inlineStr">
+        <is>
+          <t>PRTB</t>
+        </is>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -3184,6 +4158,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K55" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M55" t="n">
+        <v>70000000670</v>
+      </c>
+      <c r="N55" t="inlineStr">
+        <is>
+          <t>PR</t>
+        </is>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -3234,6 +4226,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K56" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M56" t="n">
+        <v>70000000671</v>
+      </c>
+      <c r="N56" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -3284,6 +4294,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K57" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M57" t="n">
+        <v>70000000672</v>
+      </c>
+      <c r="N57" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3334,6 +4362,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K58" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M58" t="n">
+        <v>70000000673</v>
+      </c>
+      <c r="N58" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3384,6 +4430,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K59" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M59" t="n">
+        <v>70000000674</v>
+      </c>
+      <c r="N59" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3434,6 +4498,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K60" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M60" t="n">
+        <v>70000000675</v>
+      </c>
+      <c r="N60" t="inlineStr">
+        <is>
+          <t>PTB</t>
+        </is>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3484,6 +4566,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K61" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>70000000676</v>
+      </c>
+      <c r="N61" t="inlineStr">
+        <is>
+          <t>DEM</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3534,6 +4634,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K62" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>70000000813</v>
+      </c>
+      <c r="N62" t="inlineStr">
+        <is>
+          <t>PCO</t>
+        </is>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3584,6 +4702,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>70000000823</v>
+      </c>
+      <c r="N63" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3634,6 +4770,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K64" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>70000000824</v>
+      </c>
+      <c r="N64" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3684,6 +4838,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K65" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M65" t="n">
+        <v>70000000825</v>
+      </c>
+      <c r="N65" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3734,6 +4906,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K66" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>70000000826</v>
+      </c>
+      <c r="N66" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3784,6 +4974,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K67" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>70000000827</v>
+      </c>
+      <c r="N67" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3834,6 +5042,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K68" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M68" t="n">
+        <v>70000000828</v>
+      </c>
+      <c r="N68" t="inlineStr">
+        <is>
+          <t>PRB</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3884,6 +5110,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K69" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>70000000829</v>
+      </c>
+      <c r="N69" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3934,6 +5178,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K70" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
+        <v>70000000830</v>
+      </c>
+      <c r="N70" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3984,6 +5246,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K71" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
+        <v>70000000831</v>
+      </c>
+      <c r="N71" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -4034,6 +5314,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K72" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
+        <v>70000000832</v>
+      </c>
+      <c r="N72" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -4084,6 +5382,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K73" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M73" t="n">
+        <v>70000000833</v>
+      </c>
+      <c r="N73" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -4134,6 +5450,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K74" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>70000000834</v>
+      </c>
+      <c r="N74" t="inlineStr">
+        <is>
+          <t>PROS</t>
+        </is>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -4184,6 +5518,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K75" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>70000000835</v>
+      </c>
+      <c r="N75" t="inlineStr">
+        <is>
+          <t>PC do B</t>
+        </is>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -4234,6 +5586,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K76" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>70000000836</v>
+      </c>
+      <c r="N76" t="inlineStr">
+        <is>
+          <t>PSC</t>
+        </is>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -4284,6 +5654,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K77" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>70000000837</v>
+      </c>
+      <c r="N77" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -4334,6 +5722,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K78" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M78" t="n">
+        <v>70000000838</v>
+      </c>
+      <c r="N78" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -4384,6 +5790,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K79" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M79" t="n">
+        <v>70000000839</v>
+      </c>
+      <c r="N79" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -4434,6 +5858,24 @@
           <t>ENSINO MÉDIO INCOMPLETO</t>
         </is>
       </c>
+      <c r="K80" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>70000000840</v>
+      </c>
+      <c r="N80" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -4484,6 +5926,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K81" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>70000000841</v>
+      </c>
+      <c r="N81" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -4534,6 +5994,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K82" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L82" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M82" t="n">
+        <v>70000000842</v>
+      </c>
+      <c r="N82" t="inlineStr">
+        <is>
+          <t>PP</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -4584,6 +6062,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K83" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L83" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M83" t="n">
+        <v>70000000891</v>
+      </c>
+      <c r="N83" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -4634,6 +6130,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K84" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L84" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M84" t="n">
+        <v>70000000892</v>
+      </c>
+      <c r="N84" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -4684,6 +6198,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K85" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L85" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M85" t="n">
+        <v>70000000893</v>
+      </c>
+      <c r="N85" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -4734,6 +6266,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K86" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L86" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M86" t="n">
+        <v>70000000894</v>
+      </c>
+      <c r="N86" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -4784,6 +6334,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K87" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L87" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M87" t="n">
+        <v>70000000895</v>
+      </c>
+      <c r="N87" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -4834,6 +6402,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K88" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L88" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M88" t="n">
+        <v>70000000896</v>
+      </c>
+      <c r="N88" t="inlineStr">
+        <is>
+          <t>PMDB</t>
+        </is>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -4884,6 +6470,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K89" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L89" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M89" t="n">
+        <v>70000000897</v>
+      </c>
+      <c r="N89" t="inlineStr">
+        <is>
+          <t>PT do B</t>
+        </is>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -4934,6 +6538,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K90" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L90" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M90" t="n">
+        <v>70000000898</v>
+      </c>
+      <c r="N90" t="inlineStr">
+        <is>
+          <t>PRP</t>
+        </is>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -4984,6 +6606,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K91" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L91" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M91" t="n">
+        <v>70000000899</v>
+      </c>
+      <c r="N91" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -5034,6 +6674,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K92" t="inlineStr">
+        <is>
+          <t>VIÚVO(A)</t>
+        </is>
+      </c>
+      <c r="L92" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M92" t="n">
+        <v>70000000900</v>
+      </c>
+      <c r="N92" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -5084,6 +6742,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K93" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L93" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M93" t="n">
+        <v>70000000901</v>
+      </c>
+      <c r="N93" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -5134,6 +6810,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K94" t="inlineStr">
+        <is>
+          <t>SEPARADO(A) JUDICIALMENTE</t>
+        </is>
+      </c>
+      <c r="L94" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M94" t="n">
+        <v>70000000902</v>
+      </c>
+      <c r="N94" t="inlineStr">
+        <is>
+          <t>PATRIOTA</t>
+        </is>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -5184,6 +6878,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K95" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L95" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M95" t="n">
+        <v>70000000903</v>
+      </c>
+      <c r="N95" t="inlineStr">
+        <is>
+          <t>PT do B</t>
+        </is>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -5234,6 +6946,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K96" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L96" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M96" t="n">
+        <v>70000000904</v>
+      </c>
+      <c r="N96" t="inlineStr">
+        <is>
+          <t>PV</t>
+        </is>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -5284,6 +7014,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K97" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L97" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M97" t="n">
+        <v>70000000905</v>
+      </c>
+      <c r="N97" t="inlineStr">
+        <is>
+          <t>PTN</t>
+        </is>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -5334,6 +7082,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K98" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L98" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M98" t="n">
+        <v>70000000906</v>
+      </c>
+      <c r="N98" t="inlineStr">
+        <is>
+          <t>PTN</t>
+        </is>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -5384,6 +7150,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K99" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L99" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M99" t="n">
+        <v>70000000907</v>
+      </c>
+      <c r="N99" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -5434,6 +7218,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K100" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L100" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M100" t="n">
+        <v>70000000908</v>
+      </c>
+      <c r="N100" t="inlineStr">
+        <is>
+          <t>PPL</t>
+        </is>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -5484,6 +7286,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K101" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L101" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M101" t="n">
+        <v>70000000909</v>
+      </c>
+      <c r="N101" t="inlineStr">
+        <is>
+          <t>PSL</t>
+        </is>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -5534,6 +7354,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K102" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L102" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M102" t="n">
+        <v>70000000910</v>
+      </c>
+      <c r="N102" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -5584,6 +7422,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K103" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L103" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M103" t="n">
+        <v>70000000911</v>
+      </c>
+      <c r="N103" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -5634,6 +7490,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K104" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L104" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M104" t="n">
+        <v>70000000912</v>
+      </c>
+      <c r="N104" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -5684,6 +7558,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K105" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L105" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M105" t="n">
+        <v>70000000913</v>
+      </c>
+      <c r="N105" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -5734,6 +7626,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K106" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L106" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M106" t="n">
+        <v>70000000914</v>
+      </c>
+      <c r="N106" t="inlineStr">
+        <is>
+          <t>PHS</t>
+        </is>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -5784,6 +7694,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K107" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L107" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M107" t="n">
+        <v>70000000915</v>
+      </c>
+      <c r="N107" t="inlineStr">
+        <is>
+          <t>PTC</t>
+        </is>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -5834,6 +7762,24 @@
           <t>ENSINO FUNDAMENTAL COMPLETO</t>
         </is>
       </c>
+      <c r="K108" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L108" t="inlineStr">
+        <is>
+          <t>ENSINO FUNDAMENTAL COMPLETO</t>
+        </is>
+      </c>
+      <c r="M108" t="n">
+        <v>70000001061</v>
+      </c>
+      <c r="N108" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -5884,6 +7830,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K109" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L109" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M109" t="n">
+        <v>70000001062</v>
+      </c>
+      <c r="N109" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -5934,6 +7898,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K110" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L110" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M110" t="n">
+        <v>70000001063</v>
+      </c>
+      <c r="N110" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -5984,6 +7966,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K111" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L111" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M111" t="n">
+        <v>70000001064</v>
+      </c>
+      <c r="N111" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -6034,6 +8034,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K112" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L112" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M112" t="n">
+        <v>70000001065</v>
+      </c>
+      <c r="N112" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -6084,6 +8102,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K113" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L113" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M113" t="n">
+        <v>70000001066</v>
+      </c>
+      <c r="N113" t="inlineStr">
+        <is>
+          <t>PSDC</t>
+        </is>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -6134,6 +8170,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K114" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L114" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M114" t="n">
+        <v>70000001068</v>
+      </c>
+      <c r="N114" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -6184,6 +8238,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K115" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L115" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M115" t="n">
+        <v>70000001069</v>
+      </c>
+      <c r="N115" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -6234,6 +8306,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K116" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L116" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M116" t="n">
+        <v>70000001070</v>
+      </c>
+      <c r="N116" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -6284,6 +8374,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K117" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L117" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M117" t="n">
+        <v>70000001071</v>
+      </c>
+      <c r="N117" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -6334,6 +8442,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K118" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L118" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M118" t="n">
+        <v>70000001072</v>
+      </c>
+      <c r="N118" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -6384,6 +8510,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K119" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L119" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M119" t="n">
+        <v>70000001073</v>
+      </c>
+      <c r="N119" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -6434,6 +8578,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K120" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L120" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M120" t="n">
+        <v>70000001074</v>
+      </c>
+      <c r="N120" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -6484,6 +8646,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K121" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L121" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M121" t="n">
+        <v>70000001075</v>
+      </c>
+      <c r="N121" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -6534,6 +8714,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L122" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M122" t="n">
+        <v>70000001076</v>
+      </c>
+      <c r="N122" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -6584,6 +8782,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K123" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L123" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M123" t="n">
+        <v>70000001077</v>
+      </c>
+      <c r="N123" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -6634,6 +8850,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K124" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L124" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M124" t="n">
+        <v>70000001078</v>
+      </c>
+      <c r="N124" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -6684,6 +8918,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K125" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L125" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M125" t="n">
+        <v>70000001079</v>
+      </c>
+      <c r="N125" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -6734,6 +8986,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K126" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L126" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M126" t="n">
+        <v>70000001080</v>
+      </c>
+      <c r="N126" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -6784,6 +9054,24 @@
           <t>SUPERIOR INCOMPLETO</t>
         </is>
       </c>
+      <c r="K127" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L127" t="inlineStr">
+        <is>
+          <t>SUPERIOR INCOMPLETO</t>
+        </is>
+      </c>
+      <c r="M127" t="n">
+        <v>70000001081</v>
+      </c>
+      <c r="N127" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -6834,6 +9122,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K128" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L128" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M128" t="n">
+        <v>70000001082</v>
+      </c>
+      <c r="N128" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -6884,6 +9190,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K129" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L129" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M129" t="n">
+        <v>70000001083</v>
+      </c>
+      <c r="N129" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -6934,6 +9258,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K130" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L130" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M130" t="n">
+        <v>70000001084</v>
+      </c>
+      <c r="N130" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -6984,6 +9326,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K131" t="inlineStr">
+        <is>
+          <t>CASADO(A)</t>
+        </is>
+      </c>
+      <c r="L131" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M131" t="n">
+        <v>70000001085</v>
+      </c>
+      <c r="N131" t="inlineStr">
+        <is>
+          <t>PPS</t>
+        </is>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -7034,6 +9394,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K132" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L132" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M132" t="n">
+        <v>70000001282</v>
+      </c>
+      <c r="N132" t="inlineStr">
+        <is>
+          <t>PSDB</t>
+        </is>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -7084,6 +9462,24 @@
           <t>SUPERIOR COMPLETO</t>
         </is>
       </c>
+      <c r="K133" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L133" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M133" t="n">
+        <v>70000001482</v>
+      </c>
+      <c r="N133" t="inlineStr">
+        <is>
+          <t>PT</t>
+        </is>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -7134,6 +9530,24 @@
           <t>ENSINO MÉDIO COMPLETO</t>
         </is>
       </c>
+      <c r="K134" t="inlineStr">
+        <is>
+          <t>DIVORCIADO(A)</t>
+        </is>
+      </c>
+      <c r="L134" t="inlineStr">
+        <is>
+          <t>ENSINO MÉDIO COMPLETO</t>
+        </is>
+      </c>
+      <c r="M134" t="n">
+        <v>70000001483</v>
+      </c>
+      <c r="N134" t="inlineStr">
+        <is>
+          <t>PMN</t>
+        </is>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -7182,6 +9596,24 @@
       <c r="J135" t="inlineStr">
         <is>
           <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="K135" t="inlineStr">
+        <is>
+          <t>SOLTEIRO(A)</t>
+        </is>
+      </c>
+      <c r="L135" t="inlineStr">
+        <is>
+          <t>SUPERIOR COMPLETO</t>
+        </is>
+      </c>
+      <c r="M135" t="n">
+        <v>70000001484</v>
+      </c>
+      <c r="N135" t="inlineStr">
+        <is>
+          <t>PMN</t>
         </is>
       </c>
     </row>

</xml_diff>